<commit_message>
Version 2020 sans verrous
</commit_message>
<xml_diff>
--- a/AEMO_e_O-Y.xlsx
+++ b/AEMO_e_O-Y.xlsx
@@ -4,13 +4,26 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="19935" windowHeight="7695"/>
+    <workbookView windowWidth="19890" windowHeight="7125"/>
   </bookViews>
   <sheets>
     <sheet name="MOIS" sheetId="1" r:id="rId1"/>
     <sheet name="ANNEE" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -305,18 +318,18 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="8">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="dd"/>
-    <numFmt numFmtId="179" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="180" formatCode="mmmm"/>
-    <numFmt numFmtId="181" formatCode="dddd"/>
+    <numFmt numFmtId="181" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="182" formatCode="dd"/>
+    <numFmt numFmtId="183" formatCode="dddd"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -360,8 +373,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -375,17 +412,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -399,14 +430,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -414,30 +437,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -459,39 +459,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -505,7 +490,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -541,7 +547,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -553,7 +583,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -565,19 +595,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -589,103 +655,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -703,19 +673,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -933,26 +939,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -972,17 +978,26 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -997,160 +1012,151 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="19" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="20" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="19" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="21" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="20" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="6" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="23" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1165,27 +1171,27 @@
     <xf numFmtId="180" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="181" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="183" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyProtection="1">
@@ -1288,61 +1294,61 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="181" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Check Cell" xfId="7" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="8" builtinId="17"/>
-    <cellStyle name="Note" xfId="9" builtinId="10"/>
-    <cellStyle name="Hyperlink" xfId="10" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="11" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
+    <cellStyle name="Virgule" xfId="1" builtinId="3"/>
+    <cellStyle name="Monétaire" xfId="2" builtinId="4"/>
+    <cellStyle name="Pourcentage" xfId="3" builtinId="5"/>
+    <cellStyle name="Milliers [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Monétaire [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Lien hypertexte" xfId="6" builtinId="8"/>
+    <cellStyle name="Lien hypertexte visité" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Avertissement" xfId="9" builtinId="11"/>
+    <cellStyle name="Titre" xfId="10" builtinId="15"/>
+    <cellStyle name="CTexte explicatif" xfId="11" builtinId="53"/>
+    <cellStyle name="Titre 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Titre 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Titre 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Titre 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Entrée" xfId="16" builtinId="20"/>
+    <cellStyle name="Sortie" xfId="17" builtinId="21"/>
+    <cellStyle name="Calcul" xfId="18" builtinId="22"/>
+    <cellStyle name="Vérification de cellule" xfId="19" builtinId="23"/>
+    <cellStyle name="Cellule liée" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Satisfaisant" xfId="22" builtinId="26"/>
+    <cellStyle name="Insatisfaisant" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutre" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20 % - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40 % - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60 % - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20 % - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40 % - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60 % - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20 % - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40 % - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60 % - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20 % - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40 % - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60 % - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20 % - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40 % - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60 % - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20 % - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40 % - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60 % - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -1690,7 +1696,7 @@
   <dimension ref="A1:AR300"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P301" sqref="P301"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
@@ -1732,7 +1738,7 @@
       <c r="C1" s="20"/>
       <c r="D1" s="21" t="str">
         <f ca="1">PROPER(TEXT(TODAY(),"mmmm"))</f>
-        <v>November</v>
+        <v>March</v>
       </c>
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
@@ -1796,31 +1802,31 @@
       <c r="C3" s="25"/>
       <c r="D3" s="26">
         <f ca="1">$B$12-$B$14+1</f>
-        <v>44501</v>
+        <v>45712</v>
       </c>
       <c r="E3" s="27">
         <f ca="1" t="shared" ref="E3:J3" si="0">D3+1</f>
-        <v>44502</v>
+        <v>45713</v>
       </c>
       <c r="F3" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>44503</v>
+        <v>45714</v>
       </c>
       <c r="G3" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>44504</v>
+        <v>45715</v>
       </c>
       <c r="H3" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>44505</v>
+        <v>45716</v>
       </c>
       <c r="I3" s="27">
         <f ca="1" t="shared" si="0"/>
-        <v>44506</v>
+        <v>45717</v>
       </c>
       <c r="J3" s="44">
         <f ca="1" t="shared" si="0"/>
-        <v>44507</v>
+        <v>45718</v>
       </c>
       <c r="K3" s="38"/>
       <c r="L3" s="34"/>
@@ -1844,31 +1850,31 @@
       <c r="C4" s="29"/>
       <c r="D4" s="30" t="str">
         <f ca="1">IF(OR(D3&lt;$B$4,D3&lt;$B$12,D3&gt;$B$13),"Blanc",IF(MOD(D3,$B$3)=MOD($B$5,$B$3),"Ovulation",IF(OR(AND(D3&gt;$B$5,D3&lt;=($B$5+2)),AND(D3&gt;($B$5+$B$3),D3&lt;=($B$5+$B$3+2)),AND(D3&gt;=($B$5-5),D3&lt;$B$5),AND(D3&gt;=($B$5+$B$3-5),D3&lt;($B$5+$B$3))),"Zone féconde",IF(OR(D3=($B$5+3),D3=($B$5+$B$3+3),D3=($B$5-6),D3=($B$5+$B$3-6)),"On ne sait Jamais",IF(OR(AND(D3&gt;=($B$9-$B$3+5),D3&lt;($B$6-1)),AND(D3&gt;=($B$9-$B$3+$B$3+5),D3&lt;($B$6+$B$3-1)),AND(D3&gt;($B$7+1),D3&lt;=$B$8),AND(D3&gt;($B$7+$B$3+1),D3&lt;=($B$8+$B$3))),"Période sensée inféconde",IF(OR(AND(D3&gt;=($B$9-$B$3),D3&lt;=($B$9-$B$3+4)),AND(D3&gt;=($B$9),D3&lt;=($B$9+4))),"Période prévue des règles","Imprévue"))))))</f>
-        <v>Période sensée inféconde</v>
+        <v>Blanc</v>
       </c>
       <c r="E4" s="31" t="str">
         <f ca="1" t="shared" ref="E4:J4" si="1">IF(OR(E3&lt;$B$4,E3&lt;$B$12,E3&gt;$B$13),"Blanc",IF(MOD(E3,$B$3)=MOD($B$5,$B$3),"Ovulation",IF(OR(AND(E3&gt;$B$5,E3&lt;=($B$5+2)),AND(E3&gt;($B$5+$B$3),E3&lt;=($B$5+$B$3+2)),AND(E3&gt;=($B$5-5),E3&lt;$B$5),AND(E3&gt;=($B$5+$B$3-5),E3&lt;($B$5+$B$3))),"Zone féconde",IF(OR(E3=($B$5+3),E3=($B$5+$B$3+3),E3=($B$5-6),E3=($B$5+$B$3-6)),"On ne sait Jamais",IF(OR(AND(E3&gt;=($B$9-$B$3+5),E3&lt;($B$6-1)),AND(E3&gt;=($B$9-$B$3+$B$3+5),E3&lt;($B$6+$B$3-1)),AND(E3&gt;($B$7+1),E3&lt;=$B$8),AND(E3&gt;($B$7+$B$3+1),E3&lt;=($B$8+$B$3))),"Période sensée inféconde",IF(OR(AND(E3&gt;=($B$9-$B$3),E3&lt;=($B$9-$B$3+4)),AND(E3&gt;=($B$9),E3&lt;=($B$9+4))),"Période prévue des règles","Imprévue"))))))</f>
-        <v>Période sensée inféconde</v>
+        <v>Blanc</v>
       </c>
       <c r="F4" s="31" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Période sensée inféconde</v>
+        <v>Blanc</v>
       </c>
       <c r="G4" s="31" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>On ne sait Jamais</v>
+        <v>Blanc</v>
       </c>
       <c r="H4" s="31" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Zone féconde</v>
+        <v>Blanc</v>
       </c>
       <c r="I4" s="31" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Zone féconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="J4" s="46" t="str">
         <f ca="1" t="shared" si="1"/>
-        <v>Zone féconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="K4" s="38"/>
       <c r="L4" s="42"/>
@@ -1885,36 +1891,36 @@
       </c>
       <c r="B5" s="32">
         <f ca="1">B9-14</f>
-        <v>44510</v>
+        <v>44630</v>
       </c>
       <c r="C5" s="22"/>
       <c r="D5" s="33">
         <f ca="1">D3+7</f>
-        <v>44508</v>
+        <v>45719</v>
       </c>
       <c r="E5" s="34">
         <f ca="1" t="shared" ref="E5:J5" si="2">D5+1</f>
-        <v>44509</v>
+        <v>45720</v>
       </c>
       <c r="F5" s="34">
         <f ca="1" t="shared" si="2"/>
-        <v>44510</v>
+        <v>45721</v>
       </c>
       <c r="G5" s="34">
         <f ca="1" t="shared" si="2"/>
-        <v>44511</v>
+        <v>45722</v>
       </c>
       <c r="H5" s="34">
         <f ca="1" t="shared" si="2"/>
-        <v>44512</v>
+        <v>45723</v>
       </c>
       <c r="I5" s="34">
         <f ca="1" t="shared" si="2"/>
-        <v>44513</v>
+        <v>45724</v>
       </c>
       <c r="J5" s="47">
         <f ca="1" t="shared" si="2"/>
-        <v>44514</v>
+        <v>45725</v>
       </c>
       <c r="K5" s="38"/>
       <c r="L5" s="34"/>
@@ -1931,36 +1937,36 @@
       </c>
       <c r="B6" s="22">
         <f ca="1">$B$5-5</f>
-        <v>44505</v>
+        <v>44625</v>
       </c>
       <c r="C6" s="22"/>
       <c r="D6" s="30" t="str">
         <f ca="1">IF(OR(D5&lt;$B$4,D5&lt;$B$12,D5&gt;$B$13),"Blanc",IF(MOD(D5,$B$3)=MOD($B$5,$B$3),"Ovulation",IF(OR(AND(D5&gt;$B$5,D5&lt;=($B$5+2)),AND(D5&gt;($B$5+$B$3),D5&lt;=($B$5+$B$3+2)),AND(D5&gt;=($B$5-5),D5&lt;$B$5),AND(D5&gt;=($B$5+$B$3-5),D5&lt;($B$5+$B$3))),"Zone féconde",IF(OR(D5=($B$5+3),D5=($B$5+$B$3+3),D5=($B$5-6),D5=($B$5+$B$3-6)),"On ne sait Jamais",IF(OR(AND(D5&gt;=($B$9-$B$3+5),D5&lt;($B$6-1)),AND(D5&gt;=($B$9-$B$3+$B$3+5),D5&lt;($B$6+$B$3-1)),AND(D5&gt;($B$7+1),D5&lt;=$B$8),AND(D5&gt;($B$7+$B$3+1),D5&lt;=($B$8+$B$3))),"Période sensée inféconde",IF(OR(AND(D5&gt;=($B$9-$B$3),D5&lt;=($B$9-$B$3+4)),AND(D5&gt;=($B$9),D5&lt;=($B$9+4))),"Période prévue des règles","Imprévue"))))))</f>
-        <v>Zone féconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="E6" s="31" t="str">
         <f ca="1" t="shared" ref="E6:J6" si="3">IF(OR(E5&lt;$B$4,E5&lt;$B$12,E5&gt;$B$13),"Blanc",IF(MOD(E5,$B$3)=MOD($B$5,$B$3),"Ovulation",IF(OR(AND(E5&gt;$B$5,E5&lt;=($B$5+2)),AND(E5&gt;($B$5+$B$3),E5&lt;=($B$5+$B$3+2)),AND(E5&gt;=($B$5-5),E5&lt;$B$5),AND(E5&gt;=($B$5+$B$3-5),E5&lt;($B$5+$B$3))),"Zone féconde",IF(OR(E5=($B$5+3),E5=($B$5+$B$3+3),E5=($B$5-6),E5=($B$5+$B$3-6)),"On ne sait Jamais",IF(OR(AND(E5&gt;=($B$9-$B$3+5),E5&lt;($B$6-1)),AND(E5&gt;=($B$9-$B$3+$B$3+5),E5&lt;($B$6+$B$3-1)),AND(E5&gt;($B$7+1),E5&lt;=$B$8),AND(E5&gt;($B$7+$B$3+1),E5&lt;=($B$8+$B$3))),"Période sensée inféconde",IF(OR(AND(E5&gt;=($B$9-$B$3),E5&lt;=($B$9-$B$3+4)),AND(E5&gt;=($B$9),E5&lt;=($B$9+4))),"Période prévue des règles","Imprévue"))))))</f>
-        <v>Zone féconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="F6" s="31" t="str">
         <f ca="1" t="shared" si="3"/>
-        <v>Ovulation</v>
+        <v>Imprévue</v>
       </c>
       <c r="G6" s="31" t="str">
         <f ca="1" t="shared" si="3"/>
-        <v>Zone féconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="H6" s="31" t="str">
         <f ca="1" t="shared" si="3"/>
-        <v>Zone féconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="I6" s="31" t="str">
         <f ca="1" t="shared" si="3"/>
-        <v>On ne sait Jamais</v>
+        <v>Imprévue</v>
       </c>
       <c r="J6" s="46" t="str">
         <f ca="1" t="shared" si="3"/>
-        <v>Période sensée inféconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="K6" s="38"/>
       <c r="L6" s="31"/>
@@ -1977,36 +1983,36 @@
       </c>
       <c r="B7" s="22">
         <f ca="1">$B$5+2</f>
-        <v>44512</v>
+        <v>44632</v>
       </c>
       <c r="C7" s="22"/>
       <c r="D7" s="33">
         <f ca="1">D5+7</f>
-        <v>44515</v>
+        <v>45726</v>
       </c>
       <c r="E7" s="34">
         <f ca="1" t="shared" ref="E7:J7" si="4">D7+1</f>
-        <v>44516</v>
+        <v>45727</v>
       </c>
       <c r="F7" s="34">
         <f ca="1" t="shared" si="4"/>
-        <v>44517</v>
+        <v>45728</v>
       </c>
       <c r="G7" s="34">
         <f ca="1" t="shared" si="4"/>
-        <v>44518</v>
+        <v>45729</v>
       </c>
       <c r="H7" s="34">
         <f ca="1" t="shared" si="4"/>
-        <v>44519</v>
+        <v>45730</v>
       </c>
       <c r="I7" s="34">
         <f ca="1" t="shared" si="4"/>
-        <v>44520</v>
+        <v>45731</v>
       </c>
       <c r="J7" s="47">
         <f ca="1" t="shared" si="4"/>
-        <v>44521</v>
+        <v>45732</v>
       </c>
       <c r="K7" s="38"/>
       <c r="L7" s="34"/>
@@ -2023,36 +2029,36 @@
       </c>
       <c r="B8" s="22">
         <f ca="1">B4+((B11*B3)-1)</f>
-        <v>44523</v>
+        <v>44643</v>
       </c>
       <c r="C8" s="35"/>
       <c r="D8" s="30" t="str">
         <f ca="1">IF(OR(D7&lt;$B$4,D7&lt;$B$12,D7&gt;$B$13),"Blanc",IF(MOD(D7,$B$3)=MOD($B$5,$B$3),"Ovulation",IF(OR(AND(D7&gt;$B$5,D7&lt;=($B$5+2)),AND(D7&gt;($B$5+$B$3),D7&lt;=($B$5+$B$3+2)),AND(D7&gt;=($B$5-5),D7&lt;$B$5),AND(D7&gt;=($B$5+$B$3-5),D7&lt;($B$5+$B$3))),"Zone féconde",IF(OR(D7=($B$5+3),D7=($B$5+$B$3+3),D7=($B$5-6),D7=($B$5+$B$3-6)),"On ne sait Jamais",IF(OR(AND(D7&gt;=($B$9-$B$3+5),D7&lt;($B$6-1)),AND(D7&gt;=($B$9-$B$3+$B$3+5),D7&lt;($B$6+$B$3-1)),AND(D7&gt;($B$7+1),D7&lt;=$B$8),AND(D7&gt;($B$7+$B$3+1),D7&lt;=($B$8+$B$3))),"Période sensée inféconde",IF(OR(AND(D7&gt;=($B$9-$B$3),D7&lt;=($B$9-$B$3+4)),AND(D7&gt;=($B$9),D7&lt;=($B$9+4))),"Période prévue des règles","Imprévue"))))))</f>
-        <v>Période sensée inféconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="E8" s="31" t="str">
         <f ca="1" t="shared" ref="E8:J8" si="5">IF(OR(E7&lt;$B$4,E7&lt;$B$12,E7&gt;$B$13),"Blanc",IF(MOD(E7,$B$3)=MOD($B$5,$B$3),"Ovulation",IF(OR(AND(E7&gt;$B$5,E7&lt;=($B$5+2)),AND(E7&gt;($B$5+$B$3),E7&lt;=($B$5+$B$3+2)),AND(E7&gt;=($B$5-5),E7&lt;$B$5),AND(E7&gt;=($B$5+$B$3-5),E7&lt;($B$5+$B$3))),"Zone féconde",IF(OR(E7=($B$5+3),E7=($B$5+$B$3+3),E7=($B$5-6),E7=($B$5+$B$3-6)),"On ne sait Jamais",IF(OR(AND(E7&gt;=($B$9-$B$3+5),E7&lt;($B$6-1)),AND(E7&gt;=($B$9-$B$3+$B$3+5),E7&lt;($B$6+$B$3-1)),AND(E7&gt;($B$7+1),E7&lt;=$B$8),AND(E7&gt;($B$7+$B$3+1),E7&lt;=($B$8+$B$3))),"Période sensée inféconde",IF(OR(AND(E7&gt;=($B$9-$B$3),E7&lt;=($B$9-$B$3+4)),AND(E7&gt;=($B$9),E7&lt;=($B$9+4))),"Période prévue des règles","Imprévue"))))))</f>
-        <v>Période sensée inféconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="F8" s="31" t="str">
         <f ca="1" t="shared" si="5"/>
-        <v>Période sensée inféconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="G8" s="31" t="str">
         <f ca="1" t="shared" si="5"/>
-        <v>Période sensée inféconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="H8" s="31" t="str">
         <f ca="1" t="shared" si="5"/>
-        <v>Période sensée inféconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="I8" s="31" t="str">
         <f ca="1" t="shared" si="5"/>
-        <v>Période sensée inféconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="J8" s="46" t="str">
         <f ca="1" t="shared" si="5"/>
-        <v>Période sensée inféconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="K8" s="38"/>
       <c r="L8" s="31"/>
@@ -2069,36 +2075,36 @@
       </c>
       <c r="B9" s="22">
         <f ca="1">B4+($B$11*B3)</f>
-        <v>44524</v>
+        <v>44644</v>
       </c>
       <c r="C9" s="22"/>
       <c r="D9" s="33">
         <f ca="1">D7+7</f>
-        <v>44522</v>
+        <v>45733</v>
       </c>
       <c r="E9" s="34">
         <f ca="1" t="shared" ref="E9:J9" si="6">D9+1</f>
-        <v>44523</v>
+        <v>45734</v>
       </c>
       <c r="F9" s="34">
         <f ca="1" t="shared" si="6"/>
-        <v>44524</v>
+        <v>45735</v>
       </c>
       <c r="G9" s="34">
         <f ca="1" t="shared" si="6"/>
-        <v>44525</v>
+        <v>45736</v>
       </c>
       <c r="H9" s="34">
         <f ca="1" t="shared" si="6"/>
-        <v>44526</v>
+        <v>45737</v>
       </c>
       <c r="I9" s="34">
         <f ca="1" t="shared" si="6"/>
-        <v>44527</v>
+        <v>45738</v>
       </c>
       <c r="J9" s="47">
         <f ca="1" t="shared" si="6"/>
-        <v>44528</v>
+        <v>45739</v>
       </c>
       <c r="K9" s="38"/>
       <c r="L9" s="34"/>
@@ -2115,36 +2121,36 @@
       </c>
       <c r="B10" s="35">
         <f ca="1">MONTH(B12)-MONTH(B4)</f>
-        <v>1</v>
+        <v>-7</v>
       </c>
       <c r="C10" s="22"/>
       <c r="D10" s="30" t="str">
         <f ca="1">IF(OR(D9&lt;$B$4,D9&lt;$B$12,D9&gt;$B$13),"Blanc",IF(MOD(D9,$B$3)=MOD($B$5,$B$3),"Ovulation",IF(OR(AND(D9&gt;$B$5,D9&lt;=($B$5+2)),AND(D9&gt;($B$5+$B$3),D9&lt;=($B$5+$B$3+2)),AND(D9&gt;=($B$5-5),D9&lt;$B$5),AND(D9&gt;=($B$5+$B$3-5),D9&lt;($B$5+$B$3))),"Zone féconde",IF(OR(D9=($B$5+3),D9=($B$5+$B$3+3),D9=($B$5-6),D9=($B$5+$B$3-6)),"On ne sait Jamais",IF(OR(AND(D9&gt;=($B$9-$B$3+5),D9&lt;($B$6-1)),AND(D9&gt;=($B$9-$B$3+$B$3+5),D9&lt;($B$6+$B$3-1)),AND(D9&gt;($B$7+1),D9&lt;=$B$8),AND(D9&gt;($B$7+$B$3+1),D9&lt;=($B$8+$B$3))),"Période sensée inféconde",IF(OR(AND(D9&gt;=($B$9-$B$3),D9&lt;=($B$9-$B$3+4)),AND(D9&gt;=($B$9),D9&lt;=($B$9+4))),"Période prévue des règles","Imprévue"))))))</f>
-        <v>Période sensée inféconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="E10" s="31" t="str">
         <f ca="1" t="shared" ref="E10:J10" si="7">IF(OR(E9&lt;$B$4,E9&lt;$B$12,E9&gt;$B$13),"Blanc",IF(MOD(E9,$B$3)=MOD($B$5,$B$3),"Ovulation",IF(OR(AND(E9&gt;$B$5,E9&lt;=($B$5+2)),AND(E9&gt;($B$5+$B$3),E9&lt;=($B$5+$B$3+2)),AND(E9&gt;=($B$5-5),E9&lt;$B$5),AND(E9&gt;=($B$5+$B$3-5),E9&lt;($B$5+$B$3))),"Zone féconde",IF(OR(E9=($B$5+3),E9=($B$5+$B$3+3),E9=($B$5-6),E9=($B$5+$B$3-6)),"On ne sait Jamais",IF(OR(AND(E9&gt;=($B$9-$B$3+5),E9&lt;($B$6-1)),AND(E9&gt;=($B$9-$B$3+$B$3+5),E9&lt;($B$6+$B$3-1)),AND(E9&gt;($B$7+1),E9&lt;=$B$8),AND(E9&gt;($B$7+$B$3+1),E9&lt;=($B$8+$B$3))),"Période sensée inféconde",IF(OR(AND(E9&gt;=($B$9-$B$3),E9&lt;=($B$9-$B$3+4)),AND(E9&gt;=($B$9),E9&lt;=($B$9+4))),"Période prévue des règles","Imprévue"))))))</f>
-        <v>Période sensée inféconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="F10" s="31" t="str">
         <f ca="1" t="shared" si="7"/>
-        <v>Période prévue des règles</v>
+        <v>Imprévue</v>
       </c>
       <c r="G10" s="31" t="str">
         <f ca="1" t="shared" si="7"/>
-        <v>Période prévue des règles</v>
+        <v>Imprévue</v>
       </c>
       <c r="H10" s="31" t="str">
         <f ca="1" t="shared" si="7"/>
-        <v>Période prévue des règles</v>
+        <v>Imprévue</v>
       </c>
       <c r="I10" s="31" t="str">
         <f ca="1" t="shared" si="7"/>
-        <v>Période prévue des règles</v>
+        <v>Imprévue</v>
       </c>
       <c r="J10" s="46" t="str">
         <f ca="1" t="shared" si="7"/>
-        <v>Période prévue des règles</v>
+        <v>Imprévue</v>
       </c>
       <c r="K10" s="38"/>
       <c r="L10" s="31"/>
@@ -2161,36 +2167,36 @@
       </c>
       <c r="B11" s="35">
         <f ca="1">IF($B$10&lt;0,12+$B$10,IF(B10=0,1,$B$10))</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C11" s="22"/>
       <c r="D11" s="33">
         <f ca="1">D9+7</f>
-        <v>44529</v>
+        <v>45740</v>
       </c>
       <c r="E11" s="34">
         <f ca="1" t="shared" ref="E11:J11" si="8">D11+1</f>
-        <v>44530</v>
+        <v>45741</v>
       </c>
       <c r="F11" s="34">
         <f ca="1" t="shared" si="8"/>
-        <v>44531</v>
+        <v>45742</v>
       </c>
       <c r="G11" s="34">
         <f ca="1" t="shared" si="8"/>
-        <v>44532</v>
+        <v>45743</v>
       </c>
       <c r="H11" s="34">
         <f ca="1" t="shared" si="8"/>
-        <v>44533</v>
+        <v>45744</v>
       </c>
       <c r="I11" s="34">
         <f ca="1" t="shared" si="8"/>
-        <v>44534</v>
+        <v>45745</v>
       </c>
       <c r="J11" s="47">
         <f ca="1" t="shared" si="8"/>
-        <v>44535</v>
+        <v>45746</v>
       </c>
       <c r="K11" s="38"/>
       <c r="L11" s="34"/>
@@ -2207,36 +2213,36 @@
       </c>
       <c r="B12" s="22">
         <f ca="1">DATE(YEAR(TODAY()),MONTH(TODAY()),1)</f>
-        <v>44501</v>
+        <v>45717</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="30" t="str">
         <f ca="1">IF(OR(D11&lt;$B$4,D11&lt;$B$12,D11&gt;$B$13),"Blanc",IF(MOD(D11,$B$3)=MOD($B$5,$B$3),"Ovulation",IF(OR(AND(D11&gt;$B$5,D11&lt;=($B$5+2)),AND(D11&gt;($B$5+$B$3),D11&lt;=($B$5+$B$3+2)),AND(D11&gt;=($B$5-5),D11&lt;$B$5),AND(D11&gt;=($B$5+$B$3-5),D11&lt;($B$5+$B$3))),"Zone féconde",IF(OR(D11=($B$5+3),D11=($B$5+$B$3+3),D11=($B$5-6),D11=($B$5+$B$3-6)),"On ne sait Jamais",IF(OR(AND(D11&gt;=($B$9-$B$3+5),D11&lt;($B$6-1)),AND(D11&gt;=($B$9-$B$3+$B$3+5),D11&lt;($B$6+$B$3-1)),AND(D11&gt;($B$7+1),D11&lt;=$B$8),AND(D11&gt;($B$7+$B$3+1),D11&lt;=($B$8+$B$3))),"Période sensée inféconde",IF(OR(AND(D11&gt;=($B$9-$B$3),D11&lt;=($B$9-$B$3+4)),AND(D11&gt;=($B$9),D11&lt;=($B$9+4))),"Période prévue des règles","Imprévue"))))))</f>
-        <v>Période sensée inféconde</v>
+        <v>Ovulation</v>
       </c>
       <c r="E12" s="31" t="str">
         <f ca="1" t="shared" ref="E12:J12" si="9">IF(OR(E11&lt;$B$4,E11&lt;$B$12,E11&gt;$B$13),"Blanc",IF(MOD(E11,$B$3)=MOD($B$5,$B$3),"Ovulation",IF(OR(AND(E11&gt;$B$5,E11&lt;=($B$5+2)),AND(E11&gt;($B$5+$B$3),E11&lt;=($B$5+$B$3+2)),AND(E11&gt;=($B$5-5),E11&lt;$B$5),AND(E11&gt;=($B$5+$B$3-5),E11&lt;($B$5+$B$3))),"Zone féconde",IF(OR(E11=($B$5+3),E11=($B$5+$B$3+3),E11=($B$5-6),E11=($B$5+$B$3-6)),"On ne sait Jamais",IF(OR(AND(E11&gt;=($B$9-$B$3+5),E11&lt;($B$6-1)),AND(E11&gt;=($B$9-$B$3+$B$3+5),E11&lt;($B$6+$B$3-1)),AND(E11&gt;($B$7+1),E11&lt;=$B$8),AND(E11&gt;($B$7+$B$3+1),E11&lt;=($B$8+$B$3))),"Période sensée inféconde",IF(OR(AND(E11&gt;=($B$9-$B$3),E11&lt;=($B$9-$B$3+4)),AND(E11&gt;=($B$9),E11&lt;=($B$9+4))),"Période prévue des règles","Imprévue"))))))</f>
-        <v>Période sensée inféconde</v>
+        <v>Imprévue</v>
       </c>
       <c r="F12" s="31" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>Blanc</v>
+        <v>Imprévue</v>
       </c>
       <c r="G12" s="31" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>Blanc</v>
+        <v>Imprévue</v>
       </c>
       <c r="H12" s="31" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>Blanc</v>
+        <v>Imprévue</v>
       </c>
       <c r="I12" s="31" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>Blanc</v>
+        <v>Imprévue</v>
       </c>
       <c r="J12" s="46" t="str">
         <f ca="1" t="shared" si="9"/>
-        <v>Blanc</v>
+        <v>Imprévue</v>
       </c>
       <c r="K12" s="38"/>
       <c r="L12" s="31"/>
@@ -2253,36 +2259,36 @@
       </c>
       <c r="B13" s="22">
         <f ca="1">EOMONTH(B12,0)</f>
-        <v>44530</v>
+        <v>45747</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="33">
         <f ca="1">D11+7</f>
-        <v>44536</v>
+        <v>45747</v>
       </c>
       <c r="E13" s="34">
         <f ca="1" t="shared" ref="E13:J13" si="10">D13+1</f>
-        <v>44537</v>
+        <v>45748</v>
       </c>
       <c r="F13" s="34">
         <f ca="1" t="shared" si="10"/>
-        <v>44538</v>
+        <v>45749</v>
       </c>
       <c r="G13" s="34">
         <f ca="1" t="shared" si="10"/>
-        <v>44539</v>
+        <v>45750</v>
       </c>
       <c r="H13" s="34">
         <f ca="1" t="shared" si="10"/>
-        <v>44540</v>
+        <v>45751</v>
       </c>
       <c r="I13" s="34">
         <f ca="1" t="shared" si="10"/>
-        <v>44541</v>
+        <v>45752</v>
       </c>
       <c r="J13" s="47">
         <f ca="1" t="shared" si="10"/>
-        <v>44542</v>
+        <v>45753</v>
       </c>
       <c r="K13" s="38"/>
       <c r="L13" s="34"/>
@@ -2299,12 +2305,12 @@
       </c>
       <c r="B14" s="20">
         <f ca="1">WEEKDAY(B12,2)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="36" t="str">
         <f ca="1">IF(OR(D13&lt;$B$4,D13&lt;$B$12,D13&gt;$B$13),"Blanc",IF(MOD(D13,$B$3)=MOD($B$5,$B$3),"Ovulation",IF(OR(AND(D13&gt;$B$5,D13&lt;=($B$5+2)),AND(D13&gt;($B$5+$B$3),D13&lt;=($B$5+$B$3+2)),AND(D13&gt;=($B$5-5),D13&lt;$B$5),AND(D13&gt;=($B$5+$B$3-5),D13&lt;($B$5+$B$3))),"Zone féconde",IF(OR(D13=($B$5+3),D13=($B$5+$B$3+3),D13=($B$5-6),D13=($B$5+$B$3-6)),"On ne sait Jamais",IF(OR(AND(D13&gt;=($B$9-$B$3+5),D13&lt;($B$6-1)),AND(D13&gt;=($B$9-$B$3+$B$3+5),D13&lt;($B$6+$B$3-1)),AND(D13&gt;($B$7+1),D13&lt;=$B$8),AND(D13&gt;($B$7+$B$3+1),D13&lt;=($B$8+$B$3))),"Période sensée inféconde",IF(OR(AND(D13&gt;=($B$9-$B$3),D13&lt;=($B$9-$B$3+4)),AND(D13&gt;=($B$9),D13&lt;=($B$9+4))),"Période prévue des règles","Imprévue"))))))</f>
-        <v>Blanc</v>
+        <v>Imprévue</v>
       </c>
       <c r="E14" s="37" t="str">
         <f ca="1" t="shared" ref="E14:J14" si="11">IF(OR(E13&lt;$B$4,E13&lt;$B$12,E13&gt;$B$13),"Blanc",IF(MOD(E13,$B$3)=MOD($B$5,$B$3),"Ovulation",IF(OR(AND(E13&gt;$B$5,E13&lt;=($B$5+2)),AND(E13&gt;($B$5+$B$3),E13&lt;=($B$5+$B$3+2)),AND(E13&gt;=($B$5-5),E13&lt;$B$5),AND(E13&gt;=($B$5+$B$3-5),E13&lt;($B$5+$B$3))),"Zone féconde",IF(OR(E13=($B$5+3),E13=($B$5+$B$3+3),E13=($B$5-6),E13=($B$5+$B$3-6)),"On ne sait Jamais",IF(OR(AND(E13&gt;=($B$9-$B$3+5),E13&lt;($B$6-1)),AND(E13&gt;=($B$9-$B$3+$B$3+5),E13&lt;($B$6+$B$3-1)),AND(E13&gt;($B$7+1),E13&lt;=$B$8),AND(E13&gt;($B$7+$B$3+1),E13&lt;=($B$8+$B$3))),"Période sensée inféconde",IF(OR(AND(E13&gt;=($B$9-$B$3),E13&lt;=($B$9-$B$3+4)),AND(E13&gt;=($B$9),E13&lt;=($B$9+4))),"Période prévue des règles","Imprévue"))))))</f>
@@ -7208,7 +7214,7 @@
       <c r="O300" s="38"/>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="b0aJlD2v/yVcifI8ZHESlRAAfEKRrzWIEwTH60hl8BWxQo3KiQm2YhhpFbT6h2qShQP0zGBHN4qFmfEvRUIBKg==" saltValue="A4icrsfNebbvqs5jOPGesw==" spinCount="100000" sheet="1" selectLockedCells="1" objects="1" scenarios="1"/>
+  <sheetProtection selectLockedCells="1"/>
   <mergeCells count="3">
     <mergeCell ref="D1:J1"/>
     <mergeCell ref="A17:J17"/>
@@ -7284,7 +7290,7 @@
     <row r="1" spans="1:26">
       <c r="A1" s="1">
         <f ca="1">YEAR(TODAY())</f>
-        <v>2021</v>
+        <v>2025</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -9540,4 +9546,20 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<allowEditUser xmlns="https://web.wps.cn/et/2018/main" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main" hasInvisiblePropRange="0">
+  <rangeList sheetStid="1" master="" otherUserPermission="visible"/>
+  <rangeList sheetStid="2" master="" otherUserPermission="visible"/>
+</allowEditUser>
+</file>
+
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5A5607D9-04D2-4DE1-AC0E-A7772F01BC71}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="https://web.wps.cn/et/2018/main"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>